<commit_message>
created api for static one day schedule
</commit_message>
<xml_diff>
--- a/Backend/excel/Book1.xlsx
+++ b/Backend/excel/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\inhouse\Conference-management\Backend\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34999E5D-8BBC-436A-87B2-40227C771ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE76DD3E-5FCB-4C8E-A170-24C11C8A2226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D4171177-3C16-45FE-8CA6-1470FEE2BAC9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="163">
   <si>
     <t>Domain</t>
   </si>
@@ -97,6 +97,423 @@
   </si>
   <si>
     <t>12332435edef</t>
+  </si>
+  <si>
+    <t>Deep Learning for Medical Diagnosis</t>
+  </si>
+  <si>
+    <t>Ananya, Rohan, Karthik</t>
+  </si>
+  <si>
+    <t>9876543210, 8765432109, 7654321098</t>
+  </si>
+  <si>
+    <t>ananya.ai@gmail.com, rohan.ml@gmail.com, karthik.dl@gmail.com</t>
+  </si>
+  <si>
+    <t>Advances in deep learning for disease detection.</t>
+  </si>
+  <si>
+    <t>Fraud Detection using ML</t>
+  </si>
+  <si>
+    <t>Priya, Manish</t>
+  </si>
+  <si>
+    <t>9988776655, 8877665544</t>
+  </si>
+  <si>
+    <t>priya.ml@gmail.com, manish.fraud@gmail.com</t>
+  </si>
+  <si>
+    <t>Machine learning models for fraud prevention.</t>
+  </si>
+  <si>
+    <t>CyberSec</t>
+  </si>
+  <si>
+    <t>Zero Trust Security Model</t>
+  </si>
+  <si>
+    <t>Aditi, Vikas</t>
+  </si>
+  <si>
+    <t>7890123456, 6789012345</t>
+  </si>
+  <si>
+    <t>aditi.cyber@gmail.com, vikas.security@gmail.com</t>
+  </si>
+  <si>
+    <t>Implementing Zero Trust Architecture.</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Serverless Computing and Scalability</t>
+  </si>
+  <si>
+    <t>Rajesh, Neha</t>
+  </si>
+  <si>
+    <t>8901234567, 9012345678</t>
+  </si>
+  <si>
+    <t>rajesh.cloud@gmail.com, neha.serverless@gmail.com</t>
+  </si>
+  <si>
+    <t>Benefits of serverless cloud computing.</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>Smart Home Automation</t>
+  </si>
+  <si>
+    <t>Akash, Divya</t>
+  </si>
+  <si>
+    <t>7654321987, 6543219876</t>
+  </si>
+  <si>
+    <t>akash.iot@gmail.com, divya.smart@gmail.com</t>
+  </si>
+  <si>
+    <t>IoT-enabled smart home systems.</t>
+  </si>
+  <si>
+    <t>Ethical AI in Decision Making</t>
+  </si>
+  <si>
+    <t>Sanya, Arjun</t>
+  </si>
+  <si>
+    <t>9123456789, 8234567890</t>
+  </si>
+  <si>
+    <t>sanya.ethics@gmail.com, arjun.ai@gmail.com</t>
+  </si>
+  <si>
+    <t>Ethical concerns in AI-driven decisions.</t>
+  </si>
+  <si>
+    <t>Sentiment Analysis on Social Media</t>
+  </si>
+  <si>
+    <t>Rahul, Meera</t>
+  </si>
+  <si>
+    <t>8321456789, 7214567890</t>
+  </si>
+  <si>
+    <t>rahul.nlp@gmail.com, meera.analysis@gmail.com</t>
+  </si>
+  <si>
+    <t>Using ML for sentiment detection.</t>
+  </si>
+  <si>
+    <t>RGTR</t>
+  </si>
+  <si>
+    <t>qwert,tyuio</t>
+  </si>
+  <si>
+    <t>123456789, 987654321</t>
+  </si>
+  <si>
+    <t>abc@gmail.com, wer@gmail.com</t>
+  </si>
+  <si>
+    <t>dvgthb6bye4t5y5</t>
+  </si>
+  <si>
+    <t>NLP in Healthcare</t>
+  </si>
+  <si>
+    <t>Amit, Priya</t>
+  </si>
+  <si>
+    <t>9876543210, 8765432109</t>
+  </si>
+  <si>
+    <t>amit.ai@gmail.com, priya.nlp@gmail.com</t>
+  </si>
+  <si>
+    <t>NLP techniques for medical diagnosis.</t>
+  </si>
+  <si>
+    <t>Generative AI for Drug Discovery</t>
+  </si>
+  <si>
+    <t>Nisha, Karan</t>
+  </si>
+  <si>
+    <t>nisha.drugai@gmail.com, karan.genai@gmail.com</t>
+  </si>
+  <si>
+    <t>AI in drug discovery.</t>
+  </si>
+  <si>
+    <t>AI for Predictive Maintenance</t>
+  </si>
+  <si>
+    <t>Rajeev, Anjali</t>
+  </si>
+  <si>
+    <t>rajeev.maint@gmail.com, anjali.pm@gmail.com</t>
+  </si>
+  <si>
+    <t>AI in industrial maintenance.</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning in Robotics</t>
+  </si>
+  <si>
+    <t>Deepak, Meena</t>
+  </si>
+  <si>
+    <t>deepak.rl@gmail.com, meena.robotics@gmail.com</t>
+  </si>
+  <si>
+    <t>RL techniques in robotics.</t>
+  </si>
+  <si>
+    <t>Bias in AI Decision Making</t>
+  </si>
+  <si>
+    <t>Siddharth, Rohan</t>
+  </si>
+  <si>
+    <t>siddharth.bias@gmail.com, rohan.ml@gmail.com</t>
+  </si>
+  <si>
+    <t>Ethical considerations in AI.</t>
+  </si>
+  <si>
+    <t>AI-powered Medical Imaging</t>
+  </si>
+  <si>
+    <t>Anusha, Karthik</t>
+  </si>
+  <si>
+    <t>anusha.imaging@gmail.com, karthik.ai@gmail.com</t>
+  </si>
+  <si>
+    <t>AI in medical image analysis.</t>
+  </si>
+  <si>
+    <t>Deep Learning for Fraud Detection</t>
+  </si>
+  <si>
+    <t>Meera, Vikram</t>
+  </si>
+  <si>
+    <t>meera.fraud@gmail.com, vikram.ml@gmail.com</t>
+  </si>
+  <si>
+    <t>Using DL for fraud prevention.</t>
+  </si>
+  <si>
+    <t>ML for Anomaly Detection</t>
+  </si>
+  <si>
+    <t>Arjun, Sneha</t>
+  </si>
+  <si>
+    <t>arjun.ad@gmail.com, sneha.anomaly@gmail.com</t>
+  </si>
+  <si>
+    <t>Identifying anomalies using ML.</t>
+  </si>
+  <si>
+    <t>Blockchain for Security</t>
+  </si>
+  <si>
+    <t>Tarun, Neha</t>
+  </si>
+  <si>
+    <t>tarun.bc@gmail.com, neha.sec@gmail.com</t>
+  </si>
+  <si>
+    <t>Blockchain applications in cybersecurity.</t>
+  </si>
+  <si>
+    <t>AI-powered Threat Detection</t>
+  </si>
+  <si>
+    <t>Vikas, Divya</t>
+  </si>
+  <si>
+    <t>vikas.threat@gmail.com, divya.ml@gmail.com</t>
+  </si>
+  <si>
+    <t>Using AI to detect cyber threats.</t>
+  </si>
+  <si>
+    <t>Cloud Security Best Practices</t>
+  </si>
+  <si>
+    <t>Aditi, Manish</t>
+  </si>
+  <si>
+    <t>aditi.cloud@gmail.com, manish.sec@gmail.com</t>
+  </si>
+  <si>
+    <t>Enhancing cloud security.</t>
+  </si>
+  <si>
+    <t>Multi-cloud Strategy</t>
+  </si>
+  <si>
+    <t>Rohit, Sneha</t>
+  </si>
+  <si>
+    <t>rohit.multi@gmail.com, sneha.cloud@gmail.com</t>
+  </si>
+  <si>
+    <t>Managing multi-cloud environments.</t>
+  </si>
+  <si>
+    <t>IoT in Smart Cities</t>
+  </si>
+  <si>
+    <t>Aarav, Pooja</t>
+  </si>
+  <si>
+    <t>aarav.smart@gmail.com, pooja.iot@gmail.com</t>
+  </si>
+  <si>
+    <t>IoT applications in urban planning.</t>
+  </si>
+  <si>
+    <t>AI for Autonomous Vehicles</t>
+  </si>
+  <si>
+    <t>Aarav, Sonal</t>
+  </si>
+  <si>
+    <t>aarav.autoai@gmail.com, sonal.cars@gmail.com</t>
+  </si>
+  <si>
+    <t>AI in self-driving technology.</t>
+  </si>
+  <si>
+    <t>Large Language Models &amp; Applications</t>
+  </si>
+  <si>
+    <t>Neha, Vikas</t>
+  </si>
+  <si>
+    <t>neha.llm@gmail.com, vikas.ai@gmail.com</t>
+  </si>
+  <si>
+    <t>Applications of large AI models.</t>
+  </si>
+  <si>
+    <t>AI for Climate Change Prediction</t>
+  </si>
+  <si>
+    <t>rohit.climateai@gmail.com, sneha.env@gmail.com</t>
+  </si>
+  <si>
+    <t>AI in environmental monitoring.</t>
+  </si>
+  <si>
+    <t>Multimodal AI Systems</t>
+  </si>
+  <si>
+    <t>Meera, Arjun</t>
+  </si>
+  <si>
+    <t>meera.mma@gmail.com, arjun.fusion@gmail.com</t>
+  </si>
+  <si>
+    <t>AI combining text, vision, and audio.</t>
+  </si>
+  <si>
+    <t>Explainable AI</t>
+  </si>
+  <si>
+    <t>Tarun, Divya</t>
+  </si>
+  <si>
+    <t>tarun.xai@gmail.com, divya.explain@gmail.com</t>
+  </si>
+  <si>
+    <t>Understanding AI model decisions.</t>
+  </si>
+  <si>
+    <t>AI in Personalized Learning</t>
+  </si>
+  <si>
+    <t>Rahul, Pooja</t>
+  </si>
+  <si>
+    <t>rahul.eduai@gmail.com, pooja.smartlearn@gmail.com</t>
+  </si>
+  <si>
+    <t>AI-driven adaptive learning.</t>
+  </si>
+  <si>
+    <t>Few-shot &amp; Zero-shot Learning</t>
+  </si>
+  <si>
+    <t>Aditi, Karan</t>
+  </si>
+  <si>
+    <t>aditi.fewshot@gmail.com, karan.zeroai@gmail.com</t>
+  </si>
+  <si>
+    <t>AI models learning with minimal data.</t>
+  </si>
+  <si>
+    <t>AI in Quantum Computing</t>
+  </si>
+  <si>
+    <t>Siddhi, Manish</t>
+  </si>
+  <si>
+    <t>siddhi.quantum@gmail.com, manish.qai@gmail.com</t>
+  </si>
+  <si>
+    <t>AI's role in quantum computing.</t>
+  </si>
+  <si>
+    <t>Human-AI Collaboration</t>
+  </si>
+  <si>
+    <t>Sanya, Vikram</t>
+  </si>
+  <si>
+    <t>sanya.hai@gmail.com, vikram.teama@gmail.com</t>
+  </si>
+  <si>
+    <t>AI augmenting human intelligence.</t>
+  </si>
+  <si>
+    <t>Computer Vision in Healthcare</t>
+  </si>
+  <si>
+    <t>Akash, Sneha</t>
+  </si>
+  <si>
+    <t>akash.cvmed@gmail.com, sneha.vision@gmail.com</t>
+  </si>
+  <si>
+    <t>AI-powered medical image processing.</t>
+  </si>
+  <si>
+    <t>Edge AI for IoT</t>
+  </si>
+  <si>
+    <t>Rajesh, Anjali</t>
+  </si>
+  <si>
+    <t>rajesh.edge@gmail.com, anjali.iotai@gmail.com</t>
+  </si>
+  <si>
+    <t>AI on edge devices for IoT.</t>
   </si>
 </sst>
 </file>
@@ -141,11 +558,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B5C1BC-B734-45ED-B212-4F56AAF76B06}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,6 +988,880 @@
         <v>45800</v>
       </c>
     </row>
+    <row r="5" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="5">
+        <v>45807</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="5">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="5">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="3">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="5">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="5">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="5">
+        <v>45807</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="5">
+        <v>45807</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="5">
+        <v>45801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="5">
+        <v>45801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="5">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="5">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G33" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="5">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="5">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="5">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G37" s="5">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="5">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G39" s="5">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" s="5">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G41" s="5">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G42" s="5">
+        <v>45805</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{E864F4D3-FA78-4CF7-94C9-040BD575D084}"/>

</xml_diff>